<commit_message>
Algorithm ready to scrap
</commit_message>
<xml_diff>
--- a/df_for_training_recommenders/df_tweets_try.xlsx
+++ b/df_for_training_recommenders/df_tweets_try.xlsx
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>tweet_id</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -483,22 +483,22 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>1446060297798799361</t>
+          <t>1446947589463683076</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1446060297798799361</t>
+          <t>1446947589463683076</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Un sujet bouleversant lors du 20h hier de @France2tv https://t.co/x01HaROdeh</t>
+          <t>RT @lemondefr: Vidéo. Abolition de la peine de mort : le discours de Robert Badinter en 1981 https://t.co/dk4Svs7VNf</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2021-10-07 10:30:16+00:00</t>
+          <t>2021-10-09 21:16:02+00:00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -510,41 +510,41 @@
         <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>105</v>
+        <v>254</v>
       </c>
       <c r="H2" t="n">
-        <v>285</v>
+        <v>0</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>{'1446395209500200960': {'tweet_id': '1446060297798799361', 'text': "@anne_sinclair @ZohraBitan @France2tv Effectivement une ignominie, dommage si vous n'aviez pas dépenser tout votre… https://t.co/SsmwUolXe4", 'date': '2021-10-08 08:41:05+00:00', 'username': 'LOG2202', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446390272909324288': {'tweet_id': '1446060297798799361', 'text': "@anne_sinclair @ZohraBitan @France2tv Si elle le vend à un gentil et fortuné couple d'Occidentaux en mal d'enfant,… https://t.co/gwUiF1RdXL", 'date': '2021-10-08 08:21:28+00:00', 'username': 'SergioSergiSer2', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446368018481754119': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @ZohraBitan @France2tv Les afghans combattants se font livrer des jeunes garçons sur le front. Les p… https://t.co/jnASoHCzgG', 'date': '2021-10-08 06:53:02+00:00', 'username': 'evabenhamou1', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446367056429989888': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @ZohraBitan @France2tv En France nous avons des milliers d’Enfants abusés par voie institutionnelle… https://t.co/eNqd2s8tQn', 'date': '2021-10-08 06:49:13+00:00', 'username': 'evabenhamou1', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446365305480097804': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @ZohraBitan @France2tv Alors ce couple avec ses deux enfants ne pourrait il pas être accueilli en Fr… https://t.co/6LgobYozfL', 'date': '2021-10-08 06:42:15+00:00', 'username': 'berangerblandi1', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446358026269700098': {'tweet_id': '1446060297798799361', 'text': "@anne_sinclair @ZohraBitan @France2tv Je n'ai pas oublié la haine des afghans envers la France...\nhttps://t.co/vJEThTDd7H", 'date': '2021-10-08 06:13:20+00:00', 'username': 'RedFox_Fr', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446356951697403945': {'tweet_id': '1446060297798799361', 'text': "@anne_sinclair @ZohraBitan @France2tv Les talibans ont gagné la partie parce qu'ils étaient soutenus par la grande… https://t.co/gbU8dJwzRT", 'date': '2021-10-08 06:09:03+00:00', 'username': 'ablette17', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446356501120102413': {'tweet_id': '1446060297798799361', 'text': "@anne_sinclair @ZohraBitan @France2tv Aucune empathie.\n\nIls n'ont pas lutté au côté des forces armées occidentales… https://t.co/u9nx8WYgVZ", 'date': '2021-10-08 06:07:16+00:00', 'username': 'RedFox_Fr', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446353841495158809': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @ZohraBitan @France2tv Lui donner l’argent via structure internationale 😡', 'date': '2021-10-08 05:56:42+00:00', 'username': 'cyclo33', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446353163070619651': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @ZohraBitan @France2tv Je n arrive pas à y croire c est atroce 😥', 'date': '2021-10-08 05:54:00+00:00', 'username': 'BonnelEliane', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446350787018465280': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Cette famille et ce bébé ne sont pas floutés et ça me choque. Aurions-nous faut ça en France ?', 'date': '2021-10-08 05:44:34+00:00', 'username': 'SoNENYSo', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446350265930690573': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Redire encore et toujours la pratique essentielle du reportage', 'date': '2021-10-08 05:42:29+00:00', 'username': 'hervebrusini', 'retweeted_status': False, 'retweet_count': 0, 'likes': 2}, '1446347417364934668': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @ZohraBitan @France2tv Terrible reportage, mais on s’attendait à quoi de la part de ces talibans?…', 'date': '2021-10-08 05:31:10+00:00', 'username': 'kerkyra81', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446343505962545164': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @ZohraBitan @France2tv T’aurais dû vendre ton mari toi 🙀', 'date': '2021-10-08 05:15:38+00:00', 'username': 'wilfried750z', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446341264660705308': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @ZohraBitan @France2tv Quelle détresse 🥺', 'date': '2021-10-08 05:06:43+00:00', 'username': 'Loiseau36175949', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446339514763554816': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @ZohraBitan @France2tv Un peu de mal qd même avec ça. Même au bout du rouleau je ne vendrai pas mon… https://t.co/BCMvOykNOY', 'date': '2021-10-08 04:59:46+00:00', 'username': 'devncow', 'retweeted_status': False, 'retweet_count': 0, 'likes': 4}, '1446311013817667584': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Kikilo', 'date': '2021-10-08 03:06:31+00:00', 'username': 'EugeneKaroubi', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446274721729875972': {'tweet_id': '1446060297798799361', 'text': "@anne_sinclair @France2tv C'est insupportable. Ce qu'on fait les américains est une honte.\nComment ces parents vont vivre avec ça ?", 'date': '2021-10-08 00:42:18+00:00', 'username': 'saphorocoeur', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446265736306077702': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @LeaSalame @France2tv Aucune situation ne peut excuser de vendre son enfant ....', 'date': '2021-10-08 00:06:36+00:00', 'username': 'franckd38635158', 'retweeted_status': False, 'retweet_count': 0, 'likes': 1}, '1446240149847875586': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Peut on les aider? Est il trop tard?', 'date': '2021-10-07 22:24:56+00:00', 'username': 'BeauvoirFatima', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446219047020924937': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Un choc', 'date': '2021-10-07 21:01:04+00:00', 'username': 'ParatteDaniell2', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446206254850920455': {'tweet_id': '1446060297798799361', 'text': "@anne_sinclair @France2tv Quel désastre, ils ont faim, ils n'ont rien. Plus d'aide internationale, pourquoi?", 'date': '2021-10-07 20:10:15+00:00', 'username': 'potirone', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446194575425642505': {'tweet_id': '1446060297798799361', 'text': "@anne_sinclair @France2tv Alors, contente d'avoir vécu avec un violeur et un escroc aux impôts ?...", 'date': '2021-10-07 19:23:50+00:00', 'username': 'Famille02934', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446189596430241796': {'tweet_id': '1446060297798799361', 'text': "@anne_sinclair @France2tv Terrible... pourtant une solution. Leur offrir l'argent nécessaire pour qu'ils puissent g… https://t.co/Jx23EvBYB7", 'date': '2021-10-07 19:04:03+00:00', 'username': 'laurentleb', 'retweeted_status': False, 'retweet_count': 0, 'likes': 1}, '1446188337153384460': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Je vous y croyais plus intelligente pour ne pas relayer ce type de reportage bidon !!!!', 'date': '2021-10-07 18:59:03+00:00', 'username': 'j_e_paquin', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446185952548999171': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Mais c’est monstrueux !', 'date': '2021-10-07 18:49:34+00:00', 'username': 'YvetteAmaraggi', 'retweeted_status': False, 'retweet_count': 0, 'likes': 1}, '1446157262339334147': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @CG7465CaroleM @France2tv Non', 'date': '2021-10-07 16:55:34+00:00', 'username': 'ArtemisVo', 'retweeted_status': False, 'retweet_count': 0, 'likes': 1}, '1446156127587155975': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @LeaSalame @France2tv Une catastrophe mondiale', 'date': '2021-10-07 16:51:03+00:00', 'username': 'HCroise', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446155806576152577': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Ce reportage m’avait échappé… je ne puis imaginer la détresse dans laquelle ces parents d… https://t.co/2sQMgn4bFg', 'date': '2021-10-07 16:49:47+00:00', 'username': 'qant1paris', 'retweeted_status': False, 'retweet_count': 0, 'likes': 3}, '1446138559858053127': {'tweet_id': '1446060297798799361', 'text': "@anne_sinclair @LeaSalame @France2tv C'est abominable", 'date': '2021-10-07 15:41:15+00:00', 'username': 'KepenneM', 'retweeted_status': False, 'retweet_count': 0, 'likes': 2}, '1446116559223545861': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Ce qui est terrible, c’est le fait que l’occident dénonce «On»s’émeut et «On»va voir d’au… https://t.co/iDz27iy8Sx', 'date': '2021-10-07 14:13:49+00:00', 'username': 'savyjerome', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446115392972214272': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv sans commentaire quand il s’agit d’un enfant', 'date': '2021-10-07 14:09:11+00:00', 'username': 'PierreTalamon', 'retweeted_status': False, 'retweet_count': 0, 'likes': 2}, '1446098180014235660': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @Steffie43214043 @France2tv @MaryseBurgot du grand journalisme . Effroyable réalité...', 'date': '2021-10-07 13:00:47+00:00', 'username': 'cwvadw', 'retweeted_status': False, 'retweet_count': 0, 'likes': 3}, '1446094630999765008': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @LeaSalame @France2tv https://t.co/t3PjxcajZD', 'date': '2021-10-07 12:46:41+00:00', 'username': 'henrythme', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446092132578742279': {'tweet_id': '1446060297798799361', 'text': "@anne_sinclair @France2tv Dans d'autres pays c'est encore plus la misère, mais moins générateurs de pleurs .... Et… https://t.co/7sOiPt0b4x", 'date': '2021-10-07 12:36:46+00:00', 'username': 'Stephbaume', 'retweeted_status': False, 'retweet_count': 0, 'likes': 4}, '1446088736840855558': {'tweet_id': '1446060297798799361', 'text': "@anne_sinclair @LeaSalame @France2tv Quelques soient leur situation c'est inadmissible qu'il échange leur enfant contre de l'argent.", 'date': '2021-10-07 12:23:16+00:00', 'username': 'Bigbms2021', 'retweeted_status': False, 'retweet_count': 0, 'likes': 3}, '1446084348541800448': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Terrible', 'date': '2021-10-07 12:05:50+00:00', 'username': 'GanonJocelyne', 'retweeted_status': False, 'retweet_count': 0, 'likes': 2}, '1446080032674394116': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Ce reportage m a brisé le cœur  😰', 'date': '2021-10-07 11:48:41+00:00', 'username': 'africarisingtwe', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446075663925010441': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv 😥😥😥', 'date': '2021-10-07 11:31:19+00:00', 'username': 'StellaMoliner', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446068656971079683': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Bouleversant 😢', 'date': '2021-10-07 11:03:29+00:00', 'username': 'Franois91692222', 'retweeted_status': False, 'retweet_count': 0, 'likes': 1}, '1446062402102042630': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Ce qui est plus "bouleversant" encore, c\'est la #GPA réclamée par des #bobos français bis… https://t.co/OkdWDUBhmX', 'date': '2021-10-07 10:38:37+00:00', 'username': 'GoldorakSon', 'retweeted_status': False, 'retweet_count': 0, 'likes': 1}, '1446061601535188998': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Et nous pendant ce temps on se plaint d’avoir un vaccin et on met @ZemmourEric au second tour….', 'date': '2021-10-07 10:35:26+00:00', 'username': 'Concomb09900009', 'retweeted_status': False, 'retweet_count': 0, 'likes': 7}, '1446061143508889603': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Oui…🥺', 'date': '2021-10-07 10:33:37+00:00', 'username': 'MariePicasso', 'retweeted_status': False, 'retweet_count': 0, 'likes': 1}, '1446061018459824129': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Fallez  pas  gueuler  " US go  homme "     ...', 'date': '2021-10-07 10:33:07+00:00', 'username': 'PoldeLeo', 'retweeted_status': False, 'retweet_count': 0, 'likes': 1}, '1446060546877444101': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Horrible', 'date': '2021-10-07 10:31:15+00:00', 'username': 'fxv369', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, 'number of replies found': 45}</t>
+          <t>{'number of replies found': 0}</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>['1446395209500200960', '1446390272909324288', '1446368018481754119', '1446367056429989888', '1446365305480097804', '1446358026269700098', '1446356951697403945', '1446356501120102413', '1446353841495158809', '1446353163070619651', '1446350787018465280', '1446350265930690573', '1446347417364934668', '1446343505962545164', '1446341264660705308', '1446339514763554816', '1446311013817667584', '1446274721729875972', '1446265736306077702', '1446240149847875586', '1446219047020924937', '1446206254850920455', '1446194575425642505', '1446189596430241796', '1446188337153384460', '1446185952548999171', '1446157262339334147', '1446156127587155975', '1446155806576152577', '1446138559858053127', '1446116559223545861', '1446115392972214272', '1446098180014235660', '1446094630999765008', '1446092132578742279', '1446088736840855558', '1446084348541800448', '1446080032674394116', '1446075663925010441', '1446068656971079683', '1446062402102042630', '1446061601535188998', '1446061143508889603', '1446061018459824129', '1446060546877444101']</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>1444637609829994505</t>
+          <t>1446447664246239237</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1444637609829994505</t>
+          <t>1446447664246239237</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>RT @coherence_e: Le 3 octobre 1940, le régime de Vichy promulgue le premier "statut des Juifs", qui les bannit de certaines professions. C'…</t>
+          <t>RT @PatrickKanner: La parole de Robert Badinter contre tous les falsificateurs de l'Histoire. PK</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2021-10-03 12:17:00+00:00</t>
+          <t>2021-10-08 12:09:31+00:00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -556,7 +556,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>1169</v>
+        <v>105</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -575,22 +575,22 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>1444220074978594816</t>
+          <t>1446060297798799361</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1444220074978594816</t>
+          <t>1446060297798799361</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>@thomassnegaroff @Gallimard … et c’est un drôlement bon livre!</t>
+          <t>Un sujet bouleversant lors du 20h hier de @France2tv https://t.co/x01HaROdeh</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2021-10-02 08:37:52+00:00</t>
+          <t>2021-10-07 10:30:16+00:00</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -602,41 +602,41 @@
         <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>2</v>
+        <v>114</v>
       </c>
       <c r="H4" t="n">
-        <v>14</v>
+        <v>313</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>{'number of replies found': 0}</t>
+          <t>{'1446572514981912578': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @ZohraBitan @France2tv dramatique!!!', 'date': '2021-10-08 20:25:38+00:00', 'username': 'pitchounette133', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446523934040629272': {'tweet_id': '1446060297798799361', 'text': "@anne_sinclair @ZohraBitan @France2tv La faute de l'Occident ?", 'date': '2021-10-08 17:12:35+00:00', 'username': 'boche_o', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446451866527731738': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @Regnier_JM @France2tv Bouleversant de voir à quel point ces gens souffrent', 'date': '2021-10-08 12:26:13+00:00', 'username': 'RamelValerie', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446448575613972489': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Bouleversant et intolérable. Mais que peut on faire ✍️✍️✍️✍️✍️', 'date': '2021-10-08 12:13:08+00:00', 'username': 'DuboisUrsule', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446420943040098304': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Obligé ?????\nDemander à DSK qui s\'en fout plein les poches en échappant "légalement"à l\'impôt !!!', 'date': '2021-10-08 10:23:20+00:00', 'username': 'ThierryTemime', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446402458847154176': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv C’est inacceptable! J’ai si mal pour eux 😢', 'date': '2021-10-08 09:09:53+00:00', 'username': 'me_nelly', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446395209500200960': {'tweet_id': '1446060297798799361', 'text': "@anne_sinclair @ZohraBitan @France2tv Effectivement une ignominie, dommage si vous n'aviez pas dépenser tout votre… https://t.co/SsmwUolXe4", 'date': '2021-10-08 08:41:05+00:00', 'username': 'LOG2202', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446390272909324288': {'tweet_id': '1446060297798799361', 'text': "@anne_sinclair @ZohraBitan @France2tv Si elle le vend à un gentil et fortuné couple d'Occidentaux en mal d'enfant,… https://t.co/gwUiF1RdXL", 'date': '2021-10-08 08:21:28+00:00', 'username': 'SergioSergiSer2', 'retweeted_status': False, 'retweet_count': 0, 'likes': 1}, '1446368018481754119': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @ZohraBitan @France2tv Les afghans combattants se font livrer des jeunes garçons sur le front. Les p… https://t.co/jnASoHCzgG', 'date': '2021-10-08 06:53:02+00:00', 'username': 'evabenhamou1', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446367056429989888': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @ZohraBitan @France2tv En France nous avons des milliers d’Enfants abusés par voie institutionnelle… https://t.co/eNqd2s8tQn', 'date': '2021-10-08 06:49:13+00:00', 'username': 'evabenhamou1', 'retweeted_status': False, 'retweet_count': 0, 'likes': 1}, '1446365305480097804': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @ZohraBitan @France2tv Alors ce couple avec ses deux enfants ne pourrait il pas être accueilli en Fr… https://t.co/6LgobYozfL', 'date': '2021-10-08 06:42:15+00:00', 'username': 'berangerblandi1', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446358026269700098': {'tweet_id': '1446060297798799361', 'text': "@anne_sinclair @ZohraBitan @France2tv Je n'ai pas oublié la haine des afghans envers la France...\nhttps://t.co/vJEThTDd7H", 'date': '2021-10-08 06:13:20+00:00', 'username': 'RedFox_Fr', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446356951697403945': {'tweet_id': '1446060297798799361', 'text': "@anne_sinclair @ZohraBitan @France2tv Les talibans ont gagné la partie parce qu'ils étaient soutenus par la grande… https://t.co/gbU8dJwzRT", 'date': '2021-10-08 06:09:03+00:00', 'username': 'ablette17', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446356501120102413': {'tweet_id': '1446060297798799361', 'text': "@anne_sinclair @ZohraBitan @France2tv Aucune empathie.\n\nIls n'ont pas lutté au côté des forces armées occidentales… https://t.co/u9nx8WYgVZ", 'date': '2021-10-08 06:07:16+00:00', 'username': 'RedFox_Fr', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446353841495158809': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @ZohraBitan @France2tv Lui donner l’argent via structure internationale 😡', 'date': '2021-10-08 05:56:42+00:00', 'username': 'cyclo33', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446353163070619651': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @ZohraBitan @France2tv Je n arrive pas à y croire c est atroce 😥', 'date': '2021-10-08 05:54:00+00:00', 'username': 'BonnelEliane', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446350787018465280': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Cette famille et ce bébé ne sont pas floutés et ça me choque. Aurions-nous faut ça en France ?', 'date': '2021-10-08 05:44:34+00:00', 'username': 'SoNENYSo', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446350265930690573': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Redire encore et toujours la pratique essentielle du reportage', 'date': '2021-10-08 05:42:29+00:00', 'username': 'hervebrusini', 'retweeted_status': False, 'retweet_count': 0, 'likes': 2}, '1446347417364934668': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @ZohraBitan @France2tv Terrible reportage, mais on s’attendait à quoi de la part de ces talibans?…', 'date': '2021-10-08 05:31:10+00:00', 'username': 'kerkyra81', 'retweeted_status': False, 'retweet_count': 0, 'likes': 1}, '1446343505962545164': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @ZohraBitan @France2tv T’aurais dû vendre ton mari toi 🙀', 'date': '2021-10-08 05:15:38+00:00', 'username': 'wilfried750z', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446341264660705308': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @ZohraBitan @France2tv Quelle détresse 🥺', 'date': '2021-10-08 05:06:43+00:00', 'username': 'Loiseau36175949', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446339514763554816': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @ZohraBitan @France2tv Un peu de mal qd même avec ça. Même au bout du rouleau je ne vendrai pas mon… https://t.co/BCMvOykNOY', 'date': '2021-10-08 04:59:46+00:00', 'username': 'devncow', 'retweeted_status': False, 'retweet_count': 0, 'likes': 7}, '1446311013817667584': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Kikilo', 'date': '2021-10-08 03:06:31+00:00', 'username': 'EugeneKaroubi', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446274721729875972': {'tweet_id': '1446060297798799361', 'text': "@anne_sinclair @France2tv C'est insupportable. Ce qu'on fait les américains est une honte.\nComment ces parents vont vivre avec ça ?", 'date': '2021-10-08 00:42:18+00:00', 'username': 'saphorocoeur', 'retweeted_status': False, 'retweet_count': 0, 'likes': 1}, '1446265736306077702': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @LeaSalame @France2tv Aucune situation ne peut excuser de vendre son enfant ....', 'date': '2021-10-08 00:06:36+00:00', 'username': 'franckd38635158', 'retweeted_status': False, 'retweet_count': 0, 'likes': 1}, '1446240149847875586': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Peut on les aider? Est il trop tard?', 'date': '2021-10-07 22:24:56+00:00', 'username': 'BeauvoirFatima', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446219047020924937': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Un choc', 'date': '2021-10-07 21:01:04+00:00', 'username': 'ParatteDaniell2', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446206254850920455': {'tweet_id': '1446060297798799361', 'text': "@anne_sinclair @France2tv Quel désastre, ils ont faim, ils n'ont rien. Plus d'aide internationale, pourquoi?", 'date': '2021-10-07 20:10:15+00:00', 'username': 'potirone', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446194575425642505': {'tweet_id': '1446060297798799361', 'text': "@anne_sinclair @France2tv Alors, contente d'avoir vécu avec un violeur et un escroc aux impôts ?...", 'date': '2021-10-07 19:23:50+00:00', 'username': 'Famille02934', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446189596430241796': {'tweet_id': '1446060297798799361', 'text': "@anne_sinclair @France2tv Terrible... pourtant une solution. Leur offrir l'argent nécessaire pour qu'ils puissent g… https://t.co/Jx23EvBYB7", 'date': '2021-10-07 19:04:03+00:00', 'username': 'laurentleb', 'retweeted_status': False, 'retweet_count': 0, 'likes': 1}, '1446188337153384460': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Je vous y croyais plus intelligente pour ne pas relayer ce type de reportage bidon !!!!', 'date': '2021-10-07 18:59:03+00:00', 'username': 'j_e_paquin', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446185952548999171': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Mais c’est monstrueux !', 'date': '2021-10-07 18:49:34+00:00', 'username': 'YvetteAmaraggi', 'retweeted_status': False, 'retweet_count': 0, 'likes': 1}, '1446157262339334147': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @CG7465CaroleM @France2tv Non', 'date': '2021-10-07 16:55:34+00:00', 'username': 'ArtemisVo', 'retweeted_status': False, 'retweet_count': 0, 'likes': 1}, '1446156127587155975': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @LeaSalame @France2tv Une catastrophe mondiale', 'date': '2021-10-07 16:51:03+00:00', 'username': 'HCroise', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446155806576152577': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Ce reportage m’avait échappé… je ne puis imaginer la détresse dans laquelle ces parents d… https://t.co/2sQMgn4bFg', 'date': '2021-10-07 16:49:47+00:00', 'username': 'qant1paris', 'retweeted_status': False, 'retweet_count': 0, 'likes': 4}, '1446138559858053127': {'tweet_id': '1446060297798799361', 'text': "@anne_sinclair @LeaSalame @France2tv C'est abominable", 'date': '2021-10-07 15:41:15+00:00', 'username': 'KepenneM', 'retweeted_status': False, 'retweet_count': 0, 'likes': 3}, '1446116559223545861': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Ce qui est terrible, c’est le fait que l’occident dénonce «On»s’émeut et «On»va voir d’au… https://t.co/iDz27iy8Sx', 'date': '2021-10-07 14:13:49+00:00', 'username': 'savyjerome', 'retweeted_status': False, 'retweet_count': 0, 'likes': 1}, '1446115392972214272': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv sans commentaire quand il s’agit d’un enfant', 'date': '2021-10-07 14:09:11+00:00', 'username': 'PierreTalamon', 'retweeted_status': False, 'retweet_count': 0, 'likes': 2}, '1446098180014235660': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @Steffie43214043 @France2tv @MaryseBurgot du grand journalisme . Effroyable réalité...', 'date': '2021-10-07 13:00:47+00:00', 'username': 'cwvadw', 'retweeted_status': False, 'retweet_count': 0, 'likes': 3}, '1446094630999765008': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @LeaSalame @France2tv https://t.co/t3PjxcajZD', 'date': '2021-10-07 12:46:41+00:00', 'username': 'henrythme', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446092132578742279': {'tweet_id': '1446060297798799361', 'text': "@anne_sinclair @France2tv Dans d'autres pays c'est encore plus la misère, mais moins générateurs de pleurs .... Et… https://t.co/7sOiPt0b4x", 'date': '2021-10-07 12:36:46+00:00', 'username': 'Stephbaume', 'retweeted_status': False, 'retweet_count': 0, 'likes': 4}, '1446088736840855558': {'tweet_id': '1446060297798799361', 'text': "@anne_sinclair @LeaSalame @France2tv Quelques soient leur situation c'est inadmissible qu'il échange leur enfant contre de l'argent.", 'date': '2021-10-07 12:23:16+00:00', 'username': 'Bigbms2021', 'retweeted_status': False, 'retweet_count': 0, 'likes': 3}, '1446084348541800448': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Terrible', 'date': '2021-10-07 12:05:50+00:00', 'username': 'GanonJocelyne', 'retweeted_status': False, 'retweet_count': 0, 'likes': 2}, '1446080032674394116': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Ce reportage m a brisé le cœur  😰', 'date': '2021-10-07 11:48:41+00:00', 'username': 'africarisingtwe', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446075663925010441': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv 😥😥😥', 'date': '2021-10-07 11:31:19+00:00', 'username': 'StellaMoliner', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446068656971079683': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Bouleversant 😢', 'date': '2021-10-07 11:03:29+00:00', 'username': 'Franois91692222', 'retweeted_status': False, 'retweet_count': 0, 'likes': 1}, '1446062402102042630': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Ce qui est plus "bouleversant" encore, c\'est la #GPA réclamée par des #bobos français bis… https://t.co/OkdWDUBhmX', 'date': '2021-10-07 10:38:37+00:00', 'username': 'GoldorakSon', 'retweeted_status': False, 'retweet_count': 0, 'likes': 1}, '1446061601535188998': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Et nous pendant ce temps on se plaint d’avoir un vaccin et on met @ZemmourEric au second tour….', 'date': '2021-10-07 10:35:26+00:00', 'username': 'Concomb09900009', 'retweeted_status': False, 'retweet_count': 0, 'likes': 13}, '1446061143508889603': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Oui…🥺', 'date': '2021-10-07 10:33:37+00:00', 'username': 'MariePicasso', 'retweeted_status': False, 'retweet_count': 0, 'likes': 1}, '1446061018459824129': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Fallez  pas  gueuler  " US go  homme "     ...', 'date': '2021-10-07 10:33:07+00:00', 'username': 'PoldeLeo', 'retweeted_status': False, 'retweet_count': 0, 'likes': 1}, '1446060546877444101': {'tweet_id': '1446060297798799361', 'text': '@anne_sinclair @France2tv Horrible', 'date': '2021-10-07 10:31:15+00:00', 'username': 'fxv369', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, 'number of replies found': 51}</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['1446572514981912578', '1446523934040629272', '1446451866527731738', '1446448575613972489', '1446420943040098304', '1446402458847154176', '1446395209500200960', '1446390272909324288', '1446368018481754119', '1446367056429989888', '1446365305480097804', '1446358026269700098', '1446356951697403945', '1446356501120102413', '1446353841495158809', '1446353163070619651', '1446350787018465280', '1446350265930690573', '1446347417364934668', '1446343505962545164', '1446341264660705308', '1446339514763554816', '1446311013817667584', '1446274721729875972', '1446265736306077702', '1446240149847875586', '1446219047020924937', '1446206254850920455', '1446194575425642505', '1446189596430241796', '1446188337153384460', '1446185952548999171', '1446157262339334147', '1446156127587155975', '1446155806576152577', '1446138559858053127', '1446116559223545861', '1446115392972214272', '1446098180014235660', '1446094630999765008', '1446092132578742279', '1446088736840855558', '1446084348541800448', '1446080032674394116', '1446075663925010441', '1446068656971079683', '1446062402102042630', '1446061601535188998', '1446061143508889603', '1446061018459824129', '1446060546877444101']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>1443336085447356419</t>
+          <t>1444637609829994505</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1443336085447356419</t>
+          <t>1444637609829994505</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>À ne surtout pas manquer! C’est joyeux, drôle, passionnant et très réussi. 👏 @MarionVanR https://t.co/RaOVpey8aA</t>
+          <t>RT @coherence_e: Le 3 octobre 1940, le régime de Vichy promulgue le premier "statut des Juifs", qui les bannit de certaines professions. C'…</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2021-09-29 22:05:13+00:00</t>
+          <t>2021-10-03 12:17:00+00:00</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -648,10 +648,10 @@
         <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>52</v>
+        <v>1175</v>
       </c>
       <c r="H5" t="n">
-        <v>164</v>
+        <v>0</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -667,22 +667,22 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>1437704082823815170</t>
+          <t>1444220074978594816</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1437704082823815170</t>
+          <t>1444220074978594816</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Marre d’entendre débattre quotidiennement d’#EricZemmour dont on connait les propos depuis des années qu’il les a a… https://t.co/1Rp2lOSGPS</t>
+          <t>@thomassnegaroff @Gallimard … et c’est un drôlement bon livre!</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2021-09-14 09:05:39+00:00</t>
+          <t>2021-10-02 08:37:52+00:00</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -694,41 +694,41 @@
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>1751</v>
+        <v>2</v>
       </c>
       <c r="H6" t="n">
-        <v>8380</v>
+        <v>14</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>{'1445075216984682512': {'tweet_id': '1437704082823815170', 'text': "@anne_sinclair Étiez vous au courant l'ampleur des fraudes de Dsk, de son hypocrisie et de ses mensonges. Pensez vo… https://t.co/iwgSrFGbvO", 'date': '2021-10-04 17:15:54+00:00', 'username': 'Kovacs24281548', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1444787220234317835': {'tweet_id': '1437704082823815170', 'text': '@anne_sinclair La France mérite mieux que les vieilles idées de notre gauche qui pense détenir la vérité du pays.\nL… https://t.co/g4QbHAUxIE', 'date': '2021-10-03 22:11:30+00:00', 'username': 'the_folie_douce', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1444317610611519488': {'tweet_id': '1437704082823815170', 'text': '@anne_sinclair Vous n’aviez pas marre d’entendre le roi du Maroc pourtant… le discours est pourtant le même!\n\n https://t.co/2uhCQXW4ne', 'date': '2021-10-02 15:05:27+00:00', 'username': 'renardbordelais', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1444164681430618117': {'tweet_id': '1437704082823815170', 'text': '@anne_sinclair Et toi? Marre d’entendre que vous êtes victimes de dsk.vous êtes pas foutu de voir ce qu’étais votre… https://t.co/zhEKwaPkh5', 'date': '2021-10-02 04:57:45+00:00', 'username': 'ScaniaTophe', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1444160402946920449': {'tweet_id': '1437704082823815170', 'text': "@anne_sinclair C est de bonne augure pour M Zemmour qu' elle le déteste , les candidats qu' elle appuie n ont pas de chance.", 'date': '2021-10-02 04:40:45+00:00', 'username': 'Erick47388069', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1443615743816445955': {'tweet_id': '1437704082823815170', 'text': '@anne_sinclair @afalcot En ouvrant Twitter au réveil .. deux jours d’affilée genre les twit les plus vus la tête a… https://t.co/13vL2WkiOV', 'date': '2021-09-30 16:36:29+00:00', 'username': 'kesskoikouij', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1443316206367383555': {'tweet_id': '1437704082823815170', 'text': "@anne_sinclair Je préfère un Zemmour qui veut sauver la France de son Déclin qu’un DSK qui ose dire qu'il se lève c… https://t.co/nOCpkfT5AF", 'date': '2021-09-29 20:46:13+00:00', 'username': 'GMarieRoze', 'retweeted_status': False, 'retweet_count': 0, 'likes': 1}, '1443314425725919234': {'tweet_id': '1437704082823815170', 'text': '@anne_sinclair Zemmour n’est pas petainiste ! Arrêtez de faire celle qui ne comprends pas !', 'date': '2021-09-29 20:39:09+00:00', 'username': 'GMarieRoze', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, 'number of replies found': 8}</t>
+          <t>{'number of replies found': 0}</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>['1445075216984682512', '1444787220234317835', '1444317610611519488', '1444164681430618117', '1444160402946920449', '1443615743816445955', '1443316206367383555', '1443314425725919234']</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>1437699904974073861</t>
+          <t>1443336085447356419</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1437699904974073861</t>
+          <t>1443336085447356419</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>RT @Mike_Bresson: Ils sont Français pour l’éternité Quelqu’un peut expliquer à Éric Zemmour que ces soldats Français sont morts pour la Fra…</t>
+          <t>À ne surtout pas manquer! C’est joyeux, drôle, passionnant et très réussi. 👏 @MarionVanR https://t.co/RaOVpey8aA</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2021-09-14 08:49:03+00:00</t>
+          <t>2021-09-29 22:05:13+00:00</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -740,10 +740,10 @@
         <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>155</v>
+        <v>52</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>164</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -759,22 +759,22 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>1437698363319885828</t>
+          <t>1437704082823815170</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1437698363319885828</t>
+          <t>1437704082823815170</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>RT @lofejoma: Les mots de Zemmour changent de statuts… ce sont maintenant des propositions politiques à décortiquer : discours oscillant en…</t>
+          <t>Marre d’entendre débattre quotidiennement d’#EricZemmour dont on connait les propos depuis des années qu’il les a a… https://t.co/1Rp2lOSGPS</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2021-09-14 08:42:55+00:00</t>
+          <t>2021-09-14 09:05:39+00:00</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -786,41 +786,41 @@
         <v>1</v>
       </c>
       <c r="G8" t="n">
-        <v>110</v>
+        <v>1750</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>8385</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>{'number of replies found': 0}</t>
+          <t>{'1445075216984682512': {'tweet_id': '1437704082823815170', 'text': "@anne_sinclair Étiez vous au courant l'ampleur des fraudes de Dsk, de son hypocrisie et de ses mensonges. Pensez vo… https://t.co/iwgSrFGbvO", 'date': '2021-10-04 17:15:54+00:00', 'username': 'Kovacs24281548', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1444787220234317835': {'tweet_id': '1437704082823815170', 'text': '@anne_sinclair La France mérite mieux que les vieilles idées de notre gauche qui pense détenir la vérité du pays.\nL… https://t.co/g4QbHAUxIE', 'date': '2021-10-03 22:11:30+00:00', 'username': 'the_folie_douce', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1444317610611519488': {'tweet_id': '1437704082823815170', 'text': '@anne_sinclair Vous n’aviez pas marre d’entendre le roi du Maroc pourtant… le discours est pourtant le même!\n\n https://t.co/2uhCQXW4ne', 'date': '2021-10-02 15:05:27+00:00', 'username': 'renardbordelais', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1444164681430618117': {'tweet_id': '1437704082823815170', 'text': '@anne_sinclair Et toi? Marre d’entendre que vous êtes victimes de dsk.vous êtes pas foutu de voir ce qu’étais votre… https://t.co/zhEKwaPkh5', 'date': '2021-10-02 04:57:45+00:00', 'username': 'ScaniaTophe', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1444160402946920449': {'tweet_id': '1437704082823815170', 'text': "@anne_sinclair C est de bonne augure pour M Zemmour qu' elle le déteste , les candidats qu' elle appuie n ont pas de chance.", 'date': '2021-10-02 04:40:45+00:00', 'username': 'Erick47388069', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, 'number of replies found': 5}</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['1445075216984682512', '1444787220234317835', '1444317610611519488', '1444164681430618117', '1444160402946920449']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>1437668305012236289</t>
+          <t>1437699904974073861</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1437668305012236289</t>
+          <t>1437699904974073861</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Un film remarquable sur #RobertBadinter hier soir sur @France3tv A revoir en replay jusqu’en novembre je crois. Un… https://t.co/igF5xGM2m4</t>
+          <t>RT @Mike_Bresson: Ils sont Français pour l’éternité Quelqu’un peut expliquer à Éric Zemmour que ces soldats Français sont morts pour la Fra…</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2021-09-14 06:43:29+00:00</t>
+          <t>2021-09-14 08:49:03+00:00</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -832,10 +832,10 @@
         <v>1</v>
       </c>
       <c r="G9" t="n">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H9" t="n">
-        <v>883</v>
+        <v>0</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -851,25 +851,22 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>1436255753178845185</t>
+          <t>1437698363319885828</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1436255753178845185</t>
+          <t>1437698363319885828</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>RT @HeleneHPDV: #FauteuilsdOrchestre🎵 @TCEOPERA ce soir à 20h55 @France5tv
-@anne_sinclair reçoit @atharaud
-@PhilharRF dir par MW Chung
-@Flo…</t>
+          <t>RT @lofejoma: Les mots de Zemmour changent de statuts… ce sont maintenant des propositions politiques à décortiquer : discours oscillant en…</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2021-09-10 09:10:30+00:00</t>
+          <t>2021-09-14 08:42:55+00:00</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -881,7 +878,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="n">
-        <v>24</v>
+        <v>110</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -900,22 +897,22 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>1436255459300847630</t>
+          <t>1437668305012236289</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1436255459300847630</t>
+          <t>1437668305012236289</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>RT @atharaud: À ce soir, dans « Fauteuil d’orchestre »  ⁦@anne_sinclair⁩ ⁦@France5tv⁩ ⁦@PhilharRF⁩ https://t.co/faJlrajepY</t>
+          <t>Un film remarquable sur #RobertBadinter hier soir sur @France3tv A revoir en replay jusqu’en novembre je crois. Un… https://t.co/igF5xGM2m4</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2021-09-10 09:09:20+00:00</t>
+          <t>2021-09-14 06:43:29+00:00</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -927,10 +924,10 @@
         <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>9</v>
+        <v>159</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>883</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -946,22 +943,24 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>1446395685486616592</t>
+          <t>1447051071113867267</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1446395685486616592</t>
+          <t>1447051071113867267</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>@HerandiCaro Exquisite.</t>
+          <t>Imagine a world without $SHIB.
+You can't because it's too painful a thought to bare.
+Few understand this.</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2021-10-08 08:42:58+00:00</t>
+          <t>2021-10-10 04:07:14+00:00</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -970,44 +969,44 @@
         </is>
       </c>
       <c r="F12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>256</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>{'number of replies found': 0}</t>
+          <t>{'1447102543692107779': {'tweet_id': '1447051071113867267', 'text': '@leadlagreport https://t.co/mnE68y1r1i', 'date': '2021-10-10 07:31:46+00:00', 'username': 'ShiBNeverDie1', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1447099081864761346': {'tweet_id': '1447051071113867267', 'text': '@leadlagreport Bear', 'date': '2021-10-10 07:18:01+00:00', 'username': 'HartmanPharr', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, 'number of replies found': 2}</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['1447102543692107779', '1447099081864761346']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>1446395169704747008</t>
+          <t>1447011658317156354</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1446395169704747008</t>
+          <t>1447011658317156354</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>@andrewhanley_ Exquisite.</t>
+          <t>Exquisite. https://t.co/7Q19rJ8Atv</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2021-10-08 08:40:55+00:00</t>
+          <t>2021-10-10 01:30:38+00:00</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1016,13 +1015,13 @@
         </is>
       </c>
       <c r="F13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -1038,22 +1037,22 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>1446395019380809728</t>
+          <t>1447011544697606144</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1446395019380809728</t>
+          <t>1447011544697606144</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>@bstofka @miltonj99519114 Exquisite.</t>
+          <t>@jdasovic2 Few.</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2021-10-08 08:40:19+00:00</t>
+          <t>2021-10-10 01:30:11+00:00</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1068,7 +1067,7 @@
         <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -1084,22 +1083,22 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>1446308516822667265</t>
+          <t>1446989819461124096</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1446308516822667265</t>
+          <t>1446989819461124096</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>@PVCharts_TA Exquisite.</t>
+          <t>Is the sky blue? https://t.co/SR2DZr1PrG</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2021-10-08 02:56:36+00:00</t>
+          <t>2021-10-10 00:03:51+00:00</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1108,13 +1107,13 @@
         </is>
       </c>
       <c r="F15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H15" t="n">
-        <v>3</v>
+        <v>86</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
@@ -1130,23 +1129,22 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>1446307725168848957</t>
+          <t>1446970992203546630</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1446307725168848957</t>
+          <t>1446970992203546630</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Crypto traders in $SHIB be like I'm down 35% today I just need 35% to break even.
-Few understand this.</t>
+          <t>Homes in Manhattan enjoyed their busiest third quarter in over 30 years. Compared to Q3 2020, the third quarter of… https://t.co/6CWjLx4Br0</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2021-10-08 02:53:27+00:00</t>
+          <t>2021-10-09 22:49:02+00:00</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1158,42 +1156,42 @@
         <v>1</v>
       </c>
       <c r="G16" t="n">
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="H16" t="n">
-        <v>412</v>
+        <v>16</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>{'1446373405620510728': {'tweet_id': '1446307725168848957', 'text': "@leadlagreport We're with u Sir😉\nThank u for Ur Support 💓 \n#SHIBARMY", 'date': '2021-10-08 07:14:26+00:00', 'username': 'emanuelad1991', 'retweeted_status': False, 'retweet_count': 0, 'likes': 2}, '1446370110952910858': {'tweet_id': '1446307725168848957', 'text': '@leadlagreport @shibhodler 🐕#SHIB to the moon🌙🌙📈📈\n\nHurry up listing #SHIB \n@RobinhoodApp\n\nWe are now approaching th… https://t.co/JBJXsP5r28', 'date': '2021-10-08 07:01:21+00:00', 'username': 'Cryptot64909570', 'retweeted_status': False, 'retweet_count': 0, 'likes': 2}, '1446368838749204481': {'tweet_id': '1446307725168848957', 'text': '@leadlagreport A nearly perfectly dyslexic set of numbers: down 35% needs ~53.85% upside to breakeven.', 'date': '2021-10-08 06:56:18+00:00', 'username': 'cacouteau', 'retweeted_status': False, 'retweet_count': 0, 'likes': 1}, '1446360965243678747': {'tweet_id': '1446307725168848957', 'text': '@leadlagreport @shibhodler YEH DILL MAANGE MORE\n🚀🚀🚀🚀 $SHIB 🚀🚀🚀🚀\nSAY Yo Yo Yooooo.......\nGo $SHIBA Goooooo.......🚀🌙… https://t.co/kyYo60E6aR', 'date': '2021-10-08 06:25:00+00:00', 'username': 'prashan81209187', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446338003790614536': {'tweet_id': '1446307725168848957', 'text': '@leadlagreport No one should understand this.', 'date': '2021-10-08 04:53:46+00:00', 'username': 'MatuszakJulien', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446337928804847648': {'tweet_id': '1446307725168848957', 'text': '@leadlagreport They will be saying shortly,”Lord, help me break even, I need the money!!”', 'date': '2021-10-08 04:53:28+00:00', 'username': 'a_bonifas', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446336392762576903': {'tweet_id': '1446307725168848957', 'text': '@leadlagreport Yeah 35 % not enough to break even', 'date': '2021-10-08 04:47:22+00:00', 'username': 'farizoglu97', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446335299752058881': {'tweet_id': '1446307725168848957', 'text': '@leadlagreport 💎🙌🏻', 'date': '2021-10-08 04:43:01+00:00', 'username': 'DarenBlonski', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446334925947424790': {'tweet_id': '1446307725168848957', 'text': '@leadlagreport Only if you sell 🙌🏼💎', 'date': '2021-10-08 04:41:32+00:00', 'username': 'baham_e', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446334278032232449': {'tweet_id': '1446307725168848957', 'text': '@leadlagreport Exquisite 😉', 'date': '2021-10-08 04:38:58+00:00', 'username': 'FacedSchiff', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446332607566782464': {'tweet_id': '1446307725168848957', 'text': '@leadlagreport @shibhodler Guys remember you all are in to make more money for future..\nYou are not selling SHIBAIN… https://t.co/zk36A0Zn2A', 'date': '2021-10-08 04:32:19+00:00', 'username': 'RAMKI52558732', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446332188622999552': {'tweet_id': '1446307725168848957', 'text': '@leadlagreport I’m still up 300% 🤷\u200d♂️', 'date': '2021-10-08 04:30:39+00:00', 'username': 'Daveyjcty', 'retweeted_status': False, 'retweet_count': 0, 'likes': 1}, '1446330815357534208': {'tweet_id': '1446307725168848957', 'text': '@leadlagreport They fomoed in and hodling the bag now', 'date': '2021-10-08 04:25:12+00:00', 'username': 'MrNunez8', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, 'number of replies found': 13}</t>
+          <t>{'number of replies found': 0}</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>['1446373405620510728', '1446370110952910858', '1446368838749204481', '1446360965243678747', '1446338003790614536', '1446337928804847648', '1446336392762576903', '1446335299752058881', '1446334925947424790', '1446334278032232449', '1446332607566782464', '1446332188622999552', '1446330815357534208']</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>1446306602387189760</t>
+          <t>1446961976014430208</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>1446306602387189760</t>
+          <t>1446961976014430208</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>#SHIB is going to singlehandedly pay off all of our national debt.
+          <t>Gonna price my Lambo in Doge divided by Shib and make money.
 Few understand this.</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2021-10-08 02:48:59+00:00</t>
+          <t>2021-10-09 22:13:12+00:00</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1205,41 +1203,41 @@
         <v>1</v>
       </c>
       <c r="G17" t="n">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="H17" t="n">
-        <v>335</v>
+        <v>163</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>{'1446384190564544542': {'tweet_id': '1446306602387189760', 'text': '@leadlagreport https://t.co/U65siFTIQl', 'date': '2021-10-08 07:57:18+00:00', 'username': 'Mschus03', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446381773194088452': {'tweet_id': '1446306602387189760', 'text': '@leadlagreport @Rally2344 DOOOOOONT BUY.   (DBUY) https://t.co/eZ5PNszRGF', 'date': '2021-10-08 07:47:41+00:00', 'username': 'Lucky_Meatology', 'retweeted_status': True, 'retweet_count': 3, 'likes': 3}, '1446377889759440918': {'tweet_id': '1446306602387189760', 'text': '@leadlagreport 🐕#SHIB to the moon🌙🌙📈📈\n\nHurry up listing #SHIB \n@RobinhoodApp\n\nWe are now approaching the news of 41… https://t.co/JoweiM7TQi', 'date': '2021-10-08 07:32:15+00:00', 'username': 'Cryptot64909570', 'retweeted_status': False, 'retweet_count': 0, 'likes': 1}, '1446362751488700429': {'tweet_id': '1446306602387189760', 'text': '@leadlagreport #SHIB yo the moon 🚀🌕🐕 \n\n#shiba #shibainu #SHIBARMY https://t.co/YYcVehSTqD', 'date': '2021-10-08 06:32:06+00:00', 'username': 'roseguzman16', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446354453242675203': {'tweet_id': '1446306602387189760', 'text': '@leadlagreport tax collected from capital gains?', 'date': '2021-10-08 05:59:08+00:00', 'username': 'Calata_Hieronis', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446347476030607362': {'tweet_id': '1446306602387189760', 'text': '@leadlagreport dream to buy a house shib will make it happen', 'date': '2021-10-08 05:31:24+00:00', 'username': 'melvinmathew54', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446340968341516290': {'tweet_id': '1446306602387189760', 'text': "@leadlagreport Ok. You're tripping.  I'll be paying attention. Waiting for your retraction.", 'date': '2021-10-08 05:05:33+00:00', 'username': 'dreatx', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446333714011545600': {'tweet_id': '1446306602387189760', 'text': '@leadlagreport #SHIB #SHIBARMY #shibarmy1M \n#USESHIBASWAP $SHIB #ShibaArmy #SHIBARIUM #shibainu #ShibaCoin #SHIBDELETEAZERO #SHIBDELETEZERO', 'date': '2021-10-08 04:36:43+00:00', 'username': 'senmay123', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446325400481665029': {'tweet_id': '1446306602387189760', 'text': '@leadlagreport Fed finally tightening will decrease its value to 8 electrons per coin.', 'date': '2021-10-08 04:03:41+00:00', 'username': 'IDKFA3', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, '1446324904660508672': {'tweet_id': '1446306602387189760', 'text': '@leadlagreport I do have an idea on how to use crypto economic stimulus, the Fed could buy up marginal (not worthle… https://t.co/dJ5rRW4h3R', 'date': '2021-10-08 04:01:43+00:00', 'username': 'Nothindoin4', 'retweeted_status': False, 'retweet_count': 0, 'likes': 0}, 'number of replies found': 10}</t>
+          <t>{'number of replies found': 0}</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>['1446384190564544542', '1446381773194088452', '1446377889759440918', '1446362751488700429', '1446354453242675203', '1446347476030607362', '1446340968341516290', '1446333714011545600', '1446325400481665029', '1446324904660508672']</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>1446292934014423043</t>
+          <t>1446961785186172928</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>1446292934014423043</t>
+          <t>1446961785186172928</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>@AztroStock Exquisite.</t>
+          <t>Exquisite. https://t.co/nQ773QUQ6o</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2021-10-08 01:54:40+00:00</t>
+          <t>2021-10-09 22:12:27+00:00</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1248,13 +1246,13 @@
         </is>
       </c>
       <c r="F18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H18" t="n">
-        <v>2</v>
+        <v>167</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
@@ -1270,22 +1268,22 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>1446291614213853186</t>
+          <t>1446961260797509634</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>1446291614213853186</t>
+          <t>1446961260797509634</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Small caps be like https://t.co/AG0COvhiTy</t>
+          <t>@v19003 Few.</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2021-10-08 01:49:26+00:00</t>
+          <t>2021-10-09 22:10:22+00:00</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1294,13 +1292,13 @@
         </is>
       </c>
       <c r="F19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
@@ -1316,22 +1314,22 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>1446290980320202753</t>
+          <t>1446960987194675203</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>1446290980320202753</t>
+          <t>1446960987194675203</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>@sunny051488 @coleman09823704 Few.</t>
+          <t>Few understand this. https://t.co/TARKKYBxIU</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2021-10-08 01:46:55+00:00</t>
+          <t>2021-10-09 22:09:17+00:00</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1346,7 +1344,7 @@
         <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
@@ -1362,22 +1360,22 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>1446290086124040195</t>
+          <t>1446960818927587328</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1446290086124040195</t>
+          <t>1446960818927587328</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>@ElectraNation @ModeWyckoff Exquisite.</t>
+          <t>@wealthchanger1 Exquisite.</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2021-10-08 01:43:21+00:00</t>
+          <t>2021-10-09 22:08:37+00:00</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1392,7 +1390,7 @@
         <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>

</xml_diff>